<commit_message>
Merged the Requirements Doc
Signed-off-by: Scott Beddall <sbeddall@gmail.com>
</commit_message>
<xml_diff>
--- a/doc/TARS req 10192011.xlsx
+++ b/doc/TARS req 10192011.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9090"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Must Requirements" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -1317,74 +1317,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -1393,7 +1325,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="4B2525"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -1675,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>